<commit_message>
update inputs mkt factor prem
</commit_message>
<xml_diff>
--- a/data/mv_inputs/inputs_test.xlsx
+++ b/data/mv_inputs/inputs_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\mv_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\mv_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810D7265-0750-453C-8F0B-65E13C28D9C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C56FB3-85AA-427E-A76F-2B05ABAB24EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fi" sheetId="8" r:id="rId1"/>
@@ -32,10 +32,21 @@
     <definedName name="Funded_Status_Loadings">'[1]Factor Loadings'!$B$8:$B$23</definedName>
     <definedName name="Liability_OAD">[1]Control!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -192,12 +203,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,8 +229,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2864,16 +2882,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2893,7 +2911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2913,12 +2931,12 @@
         <v>88.722886355057341</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <v>25.46306899999999</v>
+        <v>23.273078999999999</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -2933,32 +2951,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4">
-        <v>15.451228999999993</v>
+        <v>12.668424</v>
       </c>
       <c r="C4">
-        <v>1.2233859699999999E-2</v>
+        <v>1.132061E-2</v>
       </c>
       <c r="D4">
-        <v>175.01580594921191</v>
+        <v>165.94323712832238</v>
       </c>
       <c r="E4">
-        <v>55.145966989785123</v>
+        <v>50.524929419595544</v>
       </c>
       <c r="F4">
-        <v>122.33860015869141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>113.20609999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
       <c r="B5">
-        <v>19.400993</v>
+        <v>16.484375</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -2986,14 +3004,14 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -3004,7 +3022,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3015,7 +3033,7 @@
         <v>0.1813578792814477</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -3026,7 +3044,7 @@
         <v>5.3061384336615877E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3037,7 +3055,7 @@
         <v>0.20140740249674263</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -3048,7 +3066,7 @@
         <v>8.3709201670707736E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -3072,14 +3090,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>23</v>
       </c>
@@ -3093,7 +3111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3110,7 +3128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3127,7 +3145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3144,7 +3162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -3174,14 +3192,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3192,7 +3210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3203,7 +3221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3214,7 +3232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3225,7 +3243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3236,7 +3254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3247,7 +3265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3258,7 +3276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3269,7 +3287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3280,7 +3298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3291,7 +3309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3302,7 +3320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3313,7 +3331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3324,7 +3342,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3348,12 +3366,12 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -3394,7 +3412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3438,7 +3456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3482,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3526,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3570,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3614,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3658,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -3702,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3746,7 +3764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -3790,7 +3808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3834,7 +3852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -3878,7 +3896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -3922,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3976,28 +3994,28 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.9428E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4005,7 +4023,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4013,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -4030,17 +4048,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -4048,67 +4066,67 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>43</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9">
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10">
-        <v>3.8999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
update tsy mkt ret for 12/29/2023
</commit_message>
<xml_diff>
--- a/data/mv_inputs/inputs_test.xlsx
+++ b/data/mv_inputs/inputs_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\mv_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Documents\UPS_MV\data\mv_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C56FB3-85AA-427E-A76F-2B05ABAB24EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFFAEAE-EB4A-4126-8DDC-B599BCD3D17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fi" sheetId="8" r:id="rId1"/>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Control"/>
@@ -2557,7 +2557,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Primitive Factor Input"/>
@@ -2584,9 +2584,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2624,7 +2624,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2730,7 +2730,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2872,7 +2872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4000,6 +4000,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -4011,8 +4012,8 @@
       <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2">
-        <v>4.9428E-2</v>
+      <c r="B2" s="1">
+        <v>4.4310000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -4049,7 +4050,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>